<commit_message>
set eval_only FLAG in IDE model
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21888" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21888" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -102,6 +102,10 @@
   </si>
   <si>
     <t>softmax optimizer, step_size = 40, 60 epochs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.8.3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -154,10 +158,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -454,10 +458,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -514,6 +518,14 @@
       </c>
       <c r="B7" s="3">
         <v>0.71899999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.65700000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -530,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -541,10 +553,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -579,10 +591,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -621,7 +633,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="4"/>

</xml_diff>

<commit_message>
IDE: evaluater from zz
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -396,6 +396,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CUDA_VISIBLE_DEVICES=4,5 python3 examples/IDE_duke_1501.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_/dukemtmc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">fix bn for resnet; new train/test loader; 256*128; 1024dim feature; </t>
     </r>
@@ -427,10 +431,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CUDA_VISIBLE_DEVICES=4,5 python3 examples/IDE_duke_1501.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_/dukemtmc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>duke</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -463,11 +463,61 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CUDA_VISIBLE_DEVICES=2,3 python baseline.py -s duke -t market --logs-dir logs/duke2market-baseline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=2,3 python baseline.py --evaluate -s duke -t market --resume logs/duke2market-baseline/checkpoint.pth.tar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unfix bn for resnet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; new train/test loader; 256*128; 1024dim feature; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>use 2048dim output feature; dataloader from zzd</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unfix_bn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>python train.py --gpu_ids 0 --name baseline_ --train_all --batchsize 32 --data_dir /home/wangzd/Downloads/DukeMTMC-reID/pytorch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>python test.py --gpu_ids 0 --name baseline_ --batchsize 32 --test_dir /home/wangzd/Downloads/DukeMTMC-reID/pytorch  --which_epoch 59</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>python train.py --gpu_ids 0 --name baseline_ --train_all --batchsize 32 --data_dir /home/wangzd/Downloads/DukeMTMC-reID/pytorch</t>
+    <t>default</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,7 +525,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,6 +561,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -532,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -551,6 +609,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1057,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1081,7 +1142,7 @@
     </row>
     <row r="2" spans="1:7" ht="48.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1271,10 +1332,10 @@
         <v>66.900000000000006</v>
       </c>
       <c r="F22">
-        <v>1.8</v>
+        <v>14.8</v>
       </c>
       <c r="G22">
-        <v>7.7</v>
+        <v>34.700000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="57">
@@ -1293,13 +1354,16 @@
       <c r="F24">
         <v>18.7</v>
       </c>
+      <c r="G24">
+        <v>42.3</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="57">
       <c r="A26" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26">
         <v>51.5</v>
@@ -1312,6 +1376,46 @@
       </c>
       <c r="G26">
         <v>45.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="F27">
+        <v>20.5</v>
+      </c>
+      <c r="G27">
+        <v>44.5</v>
+      </c>
+      <c r="H27">
+        <v>62</v>
+      </c>
+      <c r="I27">
+        <v>69.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="57">
+      <c r="A29" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29">
+        <v>45.6</v>
+      </c>
+      <c r="D29">
+        <v>66.5</v>
+      </c>
+      <c r="F29">
+        <v>16.3</v>
+      </c>
+      <c r="G29">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="H29">
+        <v>56.8</v>
+      </c>
+      <c r="I29">
+        <v>65.5</v>
       </c>
     </row>
   </sheetData>
@@ -1327,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1342,12 +1446,12 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1405,6 +1509,9 @@
       <c r="A8">
         <v>1501</v>
       </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -1415,6 +1522,41 @@
       </c>
       <c r="C9" t="s">
         <v>42</v>
+      </c>
+      <c r="E9">
+        <v>77.3</v>
+      </c>
+      <c r="F9">
+        <v>87.8</v>
+      </c>
+      <c r="G9">
+        <v>91.6</v>
+      </c>
+      <c r="H9">
+        <v>58.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <v>1501</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10">
+        <v>42.3</v>
+      </c>
+      <c r="F10">
+        <v>59.8</v>
+      </c>
+      <c r="G10">
+        <v>67.7</v>
+      </c>
+      <c r="H10">
+        <v>16.5</v>
       </c>
     </row>
   </sheetData>
@@ -1425,62 +1567,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" t="s">
         <v>61</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F4" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
-      <c r="B2">
+      <c r="B5">
         <v>1501</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
         <v>62</v>
       </c>
-      <c r="F2">
+      <c r="F5">
         <v>19.600000000000001</v>
       </c>
-      <c r="G2">
+      <c r="G5">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
         <v>63</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
         <v>64</v>
       </c>
-      <c r="F3">
+      <c r="F6">
         <v>51.9</v>
       </c>
-      <c r="G3">
+      <c r="G6">
         <v>72.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "IDE: evaluater from zz"
This reverts commit 6aa0119d733f1634937e13a3d070f1560c55e2f6.
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -396,10 +396,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CUDA_VISIBLE_DEVICES=4,5 python3 examples/IDE_duke_1501.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_/dukemtmc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">fix bn for resnet; new train/test loader; 256*128; 1024dim feature; </t>
     </r>
@@ -431,6 +427,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CUDA_VISIBLE_DEVICES=4,5 python3 examples/IDE_duke_1501.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_/dukemtmc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>duke</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -463,61 +463,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CUDA_VISIBLE_DEVICES=2,3 python baseline.py -s duke -t market --logs-dir logs/duke2market-baseline</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CUDA_VISIBLE_DEVICES=2,3 python baseline.py --evaluate -s duke -t market --resume logs/duke2market-baseline/checkpoint.pth.tar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unfix bn for resnet</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">; new train/test loader; 256*128; 1024dim feature; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>use 2048dim output feature; dataloader from zzd</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unfix_bn</t>
+    <t>python test.py --gpu_ids 0 --name baseline_ --batchsize 32 --test_dir /home/wangzd/Downloads/DukeMTMC-reID/pytorch  --which_epoch 59</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>python train.py --gpu_ids 0 --name baseline_ --train_all --batchsize 32 --data_dir /home/wangzd/Downloads/DukeMTMC-reID/pytorch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>python test.py --gpu_ids 0 --name baseline_ --batchsize 32 --test_dir /home/wangzd/Downloads/DukeMTMC-reID/pytorch  --which_epoch 59</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>default</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -525,7 +475,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,14 +511,6 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -590,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -609,9 +551,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1118,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1142,7 +1081,7 @@
     </row>
     <row r="2" spans="1:7" ht="48.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1332,10 +1271,10 @@
         <v>66.900000000000006</v>
       </c>
       <c r="F22">
-        <v>14.8</v>
+        <v>1.8</v>
       </c>
       <c r="G22">
-        <v>34.700000000000003</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="57">
@@ -1354,16 +1293,13 @@
       <c r="F24">
         <v>18.7</v>
       </c>
-      <c r="G24">
-        <v>42.3</v>
-      </c>
     </row>
     <row r="26" spans="1:9" ht="57">
       <c r="A26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
         <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>57</v>
       </c>
       <c r="C26">
         <v>51.5</v>
@@ -1376,46 +1312,6 @@
       </c>
       <c r="G26">
         <v>45.8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="F27">
-        <v>20.5</v>
-      </c>
-      <c r="G27">
-        <v>44.5</v>
-      </c>
-      <c r="H27">
-        <v>62</v>
-      </c>
-      <c r="I27">
-        <v>69.8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="57">
-      <c r="A29" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29">
-        <v>45.6</v>
-      </c>
-      <c r="D29">
-        <v>66.5</v>
-      </c>
-      <c r="F29">
-        <v>16.3</v>
-      </c>
-      <c r="G29">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="H29">
-        <v>56.8</v>
-      </c>
-      <c r="I29">
-        <v>65.5</v>
       </c>
     </row>
   </sheetData>
@@ -1431,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1446,12 +1342,12 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1509,9 +1405,6 @@
       <c r="A8">
         <v>1501</v>
       </c>
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -1522,41 +1415,6 @@
       </c>
       <c r="C9" t="s">
         <v>42</v>
-      </c>
-      <c r="E9">
-        <v>77.3</v>
-      </c>
-      <c r="F9">
-        <v>87.8</v>
-      </c>
-      <c r="G9">
-        <v>91.6</v>
-      </c>
-      <c r="H9">
-        <v>58.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10">
-        <v>1501</v>
-      </c>
-      <c r="C10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10">
-        <v>42.3</v>
-      </c>
-      <c r="F10">
-        <v>59.8</v>
-      </c>
-      <c r="G10">
-        <v>67.7</v>
-      </c>
-      <c r="H10">
-        <v>16.5</v>
       </c>
     </row>
   </sheetData>
@@ -1567,72 +1425,62 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="8" t="s">
-        <v>66</v>
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="A2" t="s">
         <v>58</v>
       </c>
-      <c r="B5">
+      <c r="B2">
         <v>1501</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="F5">
+      <c r="F2">
         <v>19.600000000000001</v>
       </c>
-      <c r="G5">
+      <c r="G2">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B3" t="s">
         <v>58</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C3" t="s">
         <v>64</v>
       </c>
-      <c r="F6">
+      <c r="F3">
         <v>51.9</v>
       </c>
-      <c r="G6">
+      <c r="G3">
         <v>72.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes for triplet loss
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="zz code" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -533,31 +534,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>duke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1501_bn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bn_PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1501_bn_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bn_PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>CUDA_VISIBLE_DEVICES=4,5 python3 examples/IDE.py --evaluate -d market1501 --resume logs/ide_/dukemtmc/model_best.pth.tar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>duke</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1501_bn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bn_PCB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>duke</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1501_bn_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bn_PCB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -656,10 +657,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -955,10 +956,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -1050,10 +1051,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
@@ -1088,10 +1089,10 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
@@ -1167,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1201,21 +1202,21 @@
     </row>
     <row r="5" spans="1:7" ht="47.25" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="54.75" customHeight="1"/>
     <row r="7" spans="1:7">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="F7" s="9" t="s">
+      <c r="D7" s="10"/>
+      <c r="F7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="C8" t="s">
@@ -1409,7 +1410,7 @@
       <c r="A26" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C26">
@@ -1448,6 +1449,15 @@
       </c>
       <c r="F28">
         <v>20.3</v>
+      </c>
+      <c r="G28">
+        <v>44.2</v>
+      </c>
+      <c r="H28">
+        <v>61.4</v>
+      </c>
+      <c r="I28">
+        <v>69.099999999999994</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="57">
@@ -1491,7 +1501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1677,13 +1687,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
         <v>77</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>78</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
       </c>
       <c r="E14">
         <v>61.5</v>
@@ -1700,13 +1710,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
         <v>80</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>81</v>
-      </c>
-      <c r="C15" t="s">
-        <v>82</v>
       </c>
       <c r="E15">
         <v>61.5</v>
@@ -1730,7 +1740,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -1738,17 +1748,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1765,7 +1775,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -1781,17 +1791,8 @@
       <c r="G5">
         <v>47</v>
       </c>
-      <c r="H5">
-        <v>63.8</v>
-      </c>
-      <c r="I5">
-        <v>70.2</v>
-      </c>
-      <c r="J5">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
change ide model to resnet when args.feature==None
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
     <sheet name="ide on duke_to_1501" sheetId="3" r:id="rId3"/>
     <sheet name="zzd code" sheetId="4" r:id="rId4"/>
     <sheet name="zz code" sheetId="5" r:id="rId5"/>
+    <sheet name="triplet on dukemtmc-reid" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -561,12 +561,77 @@
     <t>CUDA_VISIBLE_DEVICES=4,5 python3 examples/IDE.py --evaluate -d market1501 --resume logs/ide_/dukemtmc/model_best.pth.tar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>hhj code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my open-reid code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ide_triples</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my_duke_s2_trainval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reported</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reported</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=0,1 python script/experiment/train.py \
+-d '(0,)' \
+--only_test false \
+--dataset duke \
+--last_conv_stride 2 \
+--normalize_feature false \
+--trainset_part trainval \
+--exp_dir 'logs/duke_s2_trainval' \
+--steps_per_log 10 \
+--epochs_per_val 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=2,3 python3 examples/IDE_triplet.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_triplet/raw/dukemtmc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ide == resnet50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ids = 32, imgs = 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ids = 64, imgs = 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,8 +675,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,8 +702,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -633,11 +717,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE1E4E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE1E4E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE1E4E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE1E4E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE1E4E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE1E4E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE1E4E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -660,6 +789,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1168,7 +1306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -1814,4 +1952,100 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="7" max="7" width="66.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1">
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" thickBot="1">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="11">
+        <v>61.09</v>
+      </c>
+      <c r="E3" s="11">
+        <v>78.819999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="12" customHeight="1">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="12">
+        <v>54.6</v>
+      </c>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "bad update: temporary"
This reverts commit 83f43a9bb8338723b1ebac22abcf994084778c85.
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
     <sheet name="pcb" sheetId="2" r:id="rId2"/>
     <sheet name="ide on duke_to_1501" sheetId="3" r:id="rId3"/>
-    <sheet name="zzd &amp; zz code" sheetId="4" r:id="rId4"/>
-    <sheet name="triplet on dukemtmc-reid" sheetId="6" r:id="rId5"/>
+    <sheet name="zzd code" sheetId="4" r:id="rId4"/>
+    <sheet name="zz code" sheetId="5" r:id="rId5"/>
+    <sheet name="triplet on dukemtmc-reid" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -624,21 +625,6 @@
   <si>
     <t>ids = 64, imgs = 4</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zzd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zz</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rerun reported</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ids = 64, imgs = 5</t>
   </si>
 </sst>
 </file>
@@ -723,7 +709,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -752,6 +738,21 @@
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE1E4E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE1E4E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE1E4E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE1E4E5"/>
       </right>
       <top style="medium">
         <color rgb="FFE1E4E5"/>
@@ -795,8 +796,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1305,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1636,190 +1637,201 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="A1" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
+      <c r="A7">
+        <v>1501</v>
+      </c>
+      <c r="B7">
+        <v>1501</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="E7">
+        <v>89</v>
+      </c>
+      <c r="F7">
+        <v>96.3</v>
+      </c>
+      <c r="G7">
+        <v>97.6</v>
+      </c>
+      <c r="H7">
+        <v>74.099999999999994</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
         <v>1501</v>
       </c>
-      <c r="B8">
-        <v>1501</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8">
+        <v>16.5</v>
+      </c>
+      <c r="F8">
+        <v>28.5</v>
+      </c>
+      <c r="G8">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="H8">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="E8">
-        <v>89</v>
-      </c>
-      <c r="F8">
-        <v>96.3</v>
-      </c>
-      <c r="G8">
-        <v>97.6</v>
-      </c>
-      <c r="H8">
-        <v>74.099999999999994</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
-        <v>1501</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
       <c r="E9">
-        <v>16.5</v>
+        <v>77.3</v>
       </c>
       <c r="F9">
-        <v>28.5</v>
+        <v>87.8</v>
       </c>
       <c r="G9">
-        <v>34.299999999999997</v>
+        <v>91.6</v>
       </c>
       <c r="H9">
-        <v>7.5</v>
+        <v>58.8</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>57</v>
       </c>
-      <c r="B10" t="s">
-        <v>58</v>
+      <c r="B10">
+        <v>1501</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="E10">
-        <v>77.3</v>
+        <v>42.3</v>
       </c>
       <c r="F10">
-        <v>87.8</v>
+        <v>59.8</v>
       </c>
       <c r="G10">
-        <v>91.6</v>
+        <v>67.7</v>
       </c>
       <c r="H10">
-        <v>58.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11">
-        <v>1501</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11">
-        <v>42.3</v>
-      </c>
-      <c r="F11">
-        <v>59.8</v>
-      </c>
-      <c r="G11">
-        <v>67.7</v>
-      </c>
-      <c r="H11">
         <v>16.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12">
+        <v>82.9</v>
+      </c>
+      <c r="F12">
+        <v>91.2</v>
+      </c>
+      <c r="G12">
+        <v>93.4</v>
+      </c>
+      <c r="H12">
+        <v>69.7</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="B13">
+        <v>1501</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E13">
-        <v>82.9</v>
+        <v>61.5</v>
       </c>
       <c r="F13">
-        <v>91.2</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="G13">
-        <v>93.4</v>
+        <v>82.6</v>
       </c>
       <c r="H13">
-        <v>69.7</v>
+        <v>33.1</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14">
-        <v>1501</v>
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E14">
         <v>61.5</v>
@@ -1836,13 +1848,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E15">
         <v>61.5</v>
@@ -1857,107 +1869,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16">
-        <v>61.5</v>
-      </c>
-      <c r="F16">
-        <v>77.400000000000006</v>
-      </c>
-      <c r="G16">
-        <v>82.6</v>
-      </c>
-      <c r="H16">
-        <v>33.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25">
-        <v>1501</v>
-      </c>
-      <c r="C25" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="G25">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26">
-        <v>51.9</v>
-      </c>
-      <c r="G26">
-        <v>72.5</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1966,10 +1878,88 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5">
+        <v>1501</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="G5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6">
+        <v>51.9</v>
+      </c>
+      <c r="G6">
+        <v>72.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2010,12 +2000,6 @@
       <c r="B4" t="s">
         <v>95</v>
       </c>
-      <c r="D4">
-        <v>61.24</v>
-      </c>
-      <c r="E4">
-        <v>77.56</v>
-      </c>
       <c r="G4" s="6" t="s">
         <v>92</v>
       </c>
@@ -2046,29 +2030,16 @@
       <c r="D10" s="12">
         <v>54.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11">
-        <v>52.6</v>
-      </c>
-      <c r="E11">
-        <v>71.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" t="s">
         <v>95</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G11" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "bad update: temporary""
This reverts commit c6f359023c66476129c0cc717a90bb842cc9fd9c.
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -9,15 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
     <sheet name="pcb" sheetId="2" r:id="rId2"/>
     <sheet name="ide on duke_to_1501" sheetId="3" r:id="rId3"/>
-    <sheet name="zzd code" sheetId="4" r:id="rId4"/>
-    <sheet name="zz code" sheetId="5" r:id="rId5"/>
-    <sheet name="triplet on dukemtmc-reid" sheetId="6" r:id="rId6"/>
+    <sheet name="zzd &amp; zz code" sheetId="4" r:id="rId4"/>
+    <sheet name="triplet on dukemtmc-reid" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -625,6 +624,21 @@
   <si>
     <t>ids = 64, imgs = 4</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zzd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rerun reported</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ids = 64, imgs = 5</t>
   </si>
 </sst>
 </file>
@@ -709,7 +723,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -738,21 +752,6 @@
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFE1E4E5"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFE1E4E5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFE1E4E5"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFE1E4E5"/>
       </right>
       <top style="medium">
         <color rgb="FFE1E4E5"/>
@@ -796,8 +795,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1306,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1637,201 +1636,190 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="A1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>41</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>45</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>1501</v>
-      </c>
-      <c r="B7">
-        <v>1501</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7">
-        <v>89</v>
-      </c>
-      <c r="F7">
-        <v>96.3</v>
-      </c>
-      <c r="G7">
-        <v>97.6</v>
-      </c>
-      <c r="H7">
-        <v>74.099999999999994</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
         <v>1501</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>1501</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>89</v>
+      </c>
+      <c r="F8">
+        <v>96.3</v>
+      </c>
+      <c r="G8">
+        <v>97.6</v>
+      </c>
+      <c r="H8">
+        <v>74.099999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>1501</v>
+      </c>
+      <c r="B9" t="s">
         <v>57</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>16.5</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>28.5</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>34.299999999999997</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>7.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9">
-        <v>77.3</v>
-      </c>
-      <c r="F9">
-        <v>87.8</v>
-      </c>
-      <c r="G9">
-        <v>91.6</v>
-      </c>
-      <c r="H9">
-        <v>58.8</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>57</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10">
+        <v>77.3</v>
+      </c>
+      <c r="F10">
+        <v>87.8</v>
+      </c>
+      <c r="G10">
+        <v>91.6</v>
+      </c>
+      <c r="H10">
+        <v>58.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
         <v>1501</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>69</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>42.3</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>59.8</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>67.7</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>16.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12">
-        <v>82.9</v>
-      </c>
-      <c r="F12">
-        <v>91.2</v>
-      </c>
-      <c r="G12">
-        <v>93.4</v>
-      </c>
-      <c r="H12">
-        <v>69.7</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13">
-        <v>1501</v>
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E13">
-        <v>61.5</v>
+        <v>82.9</v>
       </c>
       <c r="F13">
-        <v>77.400000000000006</v>
+        <v>91.2</v>
       </c>
       <c r="G13">
-        <v>82.6</v>
+        <v>93.4</v>
       </c>
       <c r="H13">
-        <v>33.1</v>
+        <v>69.7</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="B14">
+        <v>1501</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E14">
         <v>61.5</v>
@@ -1848,13 +1836,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E15">
         <v>61.5</v>
@@ -1869,7 +1857,107 @@
         <v>33.1</v>
       </c>
     </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16">
+        <v>61.5</v>
+      </c>
+      <c r="F16">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="G16">
+        <v>82.6</v>
+      </c>
+      <c r="H16">
+        <v>33.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25">
+        <v>1501</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="G25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26">
+        <v>51.9</v>
+      </c>
+      <c r="G26">
+        <v>72.5</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1878,88 +1966,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5">
-        <v>1501</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="G5">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6">
-        <v>51.9</v>
-      </c>
-      <c r="G6">
-        <v>72.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2000,6 +2010,12 @@
       <c r="B4" t="s">
         <v>95</v>
       </c>
+      <c r="D4">
+        <v>61.24</v>
+      </c>
+      <c r="E4">
+        <v>77.56</v>
+      </c>
       <c r="G4" s="6" t="s">
         <v>92</v>
       </c>
@@ -2030,16 +2046,29 @@
       <c r="D10" s="12">
         <v>54.6</v>
       </c>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="1:7">
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>52.6</v>
+      </c>
+      <c r="E11">
+        <v>71.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
         <v>94</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>95</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New: --output_feature setting in IDE
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="129">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -799,19 +799,44 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CUDA_VISIBLE_DEVICES=6,7 python3 examples/IDE.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_new/256/basis/dukemtmc --height 384 --re 0.5  --features 256 --output_feature fc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basis, no re</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=6,7 python3 examples/IDE.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_new/2048/h_384_no_crop_re/dukemtmc --height 384 --re 0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">basis, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-s 1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>basis, -s 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CUDA_VISIBLE_DEVICES=6,7 python3 examples/IDE.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_new/256/basis/dukemtmc --height 384 --re 0.5  --features 256 --output_feature fc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>basis, no re</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CUDA_VISIBLE_DEVICES=6,7 python3 examples/IDE.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_new/2048/h_384_no_crop_re/dukemtmc --height 384 --re 0.5</t>
+    <t>CUDA_VISIBLE_DEVICES=6,7 python3 examples/IDE.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_new/256/basis_s_1/dukemtmc --height 384 --re 0.5 -s 1 --features 256 --output_feature fc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -945,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -972,14 +997,16 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1275,10 +1302,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1370,10 +1397,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1408,10 +1435,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1485,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1528,14 +1555,14 @@
     </row>
     <row r="6" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="14"/>
+      <c r="F7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
@@ -1806,10 +1833,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1826,7 +1853,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="12" t="s">
         <v>118</v>
       </c>
       <c r="C35">
@@ -1848,7 +1875,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="17" t="s">
         <v>119</v>
       </c>
       <c r="C37">
@@ -1858,28 +1885,63 @@
         <v>78.81</v>
       </c>
       <c r="F37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38">
+        <v>61.44</v>
+      </c>
+      <c r="D38">
+        <v>79.36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>120</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B39" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F38" t="s">
+      <c r="C39">
+        <v>57.87</v>
+      </c>
+      <c r="D39">
+        <v>76.38</v>
+      </c>
+      <c r="F39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40">
+        <v>59.99</v>
+      </c>
+      <c r="D40">
+        <v>77.05</v>
+      </c>
+      <c r="F40" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>124</v>
+      <c r="C41">
+        <v>51.03</v>
+      </c>
+      <c r="D41">
+        <v>70.650000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -1905,16 +1967,16 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -2141,16 +2203,16 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">

</xml_diff>

<commit_message>
update: multi fps support for myGT
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="158">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -927,6 +927,34 @@
   </si>
   <si>
     <t>CUDA_VISIBLE_DEVICES=0,1,2,3,4,5 python3 examples/get_test_feature.py  -j 24 -b 576 --resume logs/ide_new/256/basis_s_1/duke_my_gt/checkpoint.pth.tar --features 256 --output_feature fc --l0_name my_gt_fc256 -s 1 --height 384 -d detections</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basis, feat=1024, out_feat=pool5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feat=1024, out_feat=pool5, rand_crop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ide softmax 256 @ basis, -s 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30fps, 10epoch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60fps, 6epoch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1fps, 20epoch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=0,1 python3 examples/IDE.py --lr 0.01 --epochs 20 -b 192 --train -d duke_my_gt --combine-trainval --logs-dir logs/ide_new/256/basis_s_1/duke_my_gt/1_fps --height 384 --re 0.5 -s 1 --features 256 --output_feature fc --mygt_fps 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2176,10 +2204,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2573,50 +2601,84 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B39" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39">
+        <v>59.37</v>
+      </c>
+      <c r="D39">
+        <v>77.08</v>
+      </c>
+      <c r="F39">
+        <v>15.92</v>
+      </c>
+      <c r="G39">
+        <v>36.35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40">
+        <v>50.87</v>
+      </c>
+      <c r="D40">
+        <v>71.08</v>
+      </c>
+      <c r="F40">
+        <v>19.52</v>
+      </c>
+      <c r="G40">
+        <v>43.71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B41" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C39">
+      <c r="C41">
         <v>57.87</v>
       </c>
-      <c r="D39">
+      <c r="D41">
         <v>76.38</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I41" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="16" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C40">
+      <c r="C42">
         <v>59.99</v>
       </c>
-      <c r="D40">
+      <c r="D42">
         <v>77.05</v>
       </c>
-      <c r="F40">
+      <c r="F42">
         <v>14.87</v>
       </c>
-      <c r="G40">
+      <c r="G42">
         <v>36.380000000000003</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I42" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>122</v>
       </c>
-      <c r="C41">
+      <c r="C43">
         <v>51.03</v>
       </c>
-      <c r="D41">
+      <c r="D43">
         <v>70.650000000000006</v>
       </c>
     </row>
@@ -2634,10 +2696,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2645,7 +2707,7 @@
     <col min="2" max="2" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>87</v>
       </c>
@@ -2653,7 +2715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -2664,7 +2726,7 @@
         <v>74.09</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -2675,17 +2737,38 @@
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>148</v>
       </c>
       <c r="C7">
         <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2699,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updates: support for separate icam
</commit_message>
<xml_diff>
--- a/pcb_rpp_result.xlsx
+++ b/pcb_rpp_result.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hou_yz\Documents\GitHub\open-reid-PCB_n_RPP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnny\Documents\GitHub\open-reid-PCB_n_RPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03F4ED7-EC99-4DB2-8594-10B1D3570FFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="9780" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21888" windowHeight="9780" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
@@ -20,6 +21,7 @@
     <sheet name="my_gt" sheetId="7" r:id="rId6"/>
     <sheet name="get feature time" sheetId="8" r:id="rId7"/>
     <sheet name="train my_gt time" sheetId="9" r:id="rId8"/>
+    <sheet name="train camstyle time" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="191">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -170,7 +172,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -181,7 +183,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -197,7 +199,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -208,7 +210,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -224,7 +226,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -235,7 +237,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -251,7 +253,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -262,7 +264,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -278,7 +280,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -343,7 +345,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -354,7 +356,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -370,7 +372,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -381,7 +383,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -443,7 +445,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -454,7 +456,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -463,7 +465,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -690,7 +692,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -701,7 +703,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -711,7 +713,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -728,7 +730,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -739,38 +741,6 @@
   </si>
   <si>
     <t>ide softmax 256</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">basis = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>no_crop, -h 384,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> re 0.5</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -793,7 +763,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -811,10 +781,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CUDA_VISIBLE_DEVICES=6,7 python3 examples/IDE.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_new/256/basis_s_1/dukemtmc --height 384 --re 0.5 -s 1 --features 256 --output_feature fc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>openpose</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -897,7 +863,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -908,7 +874,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -934,10 +900,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CUDA_VISIBLE_DEVICES=0,1,2,3,4,5 python3 examples/get_test_feature.py  -j 24 -b 576 --resume logs/ide_new/256/basis_s_1/duke_my_gt/checkpoint.pth.tar --features 256 --output_feature fc --l0_name my_gt_fc256 -s 1 --height 384 -d detections</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>dukemtmc-reid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -950,53 +912,162 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CUDA_VISIBLE_DEVICES=4,5,6,7 python3 examples/get_test_feature.py  -j 16 -b 384 --resume logs/ide_new/256/basis_s_1/duke_my_gt/6_fps/model_best.pth.tar --features 256 --output_feature fc --l0_name fc256_6_fps -s 1 --height 384 -d detections  --det_time trainval_mini</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60fps, 6epoch, 0.01lr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">30fps, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>myGT @ fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12fps, 20epoch, 0.1lr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6fps, 40epoch, 0.1lr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>CUDA_VISIBLE_DEVICES=0,1 python3 examples/IDE.py --lr 0.1 --epochs 60 -b 192 --train -d duke_my_gt --combine-trainval --logs-dir logs/ide_new/256/basis_s_1/duke_my_gt/1_fps --height 384 --re 0.5 -s 1 --features 256 --output_feature fc --mygt_fps 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CUDA_VISIBLE_DEVICES=4,5,6,7 python3 examples/get_test_feature.py  -j 16 -b 384 --resume logs/ide_new/256/basis_s_1/duke_my_gt/6_fps/model_best.pth.tar --features 256 --output_feature fc --l0_name fc256_6_fps -s 1 --height 384 -d detections  --det_time trainval_mini</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>60fps, 6epoch, 0.01lr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">30fps, </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>myGT @ fps</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12fps, 20epoch, 0.1lr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CUDA_VISIBLE_DEVICES=0,1,2,3,4,5 python3 examples/IDE.py --lr 0.1 --epochs 20 -b 576 --train -d duke_my_gt --combine-trainval --logs-dir logs/ide_new/256/basis_s_1/duke_my_gt/12_fps --height 384 --re 0.5 -s 1 --features 256 --output_feature fc --mygt_fps 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6fps, 40epoch, 0.1lr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch time</t>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=0,1 python main.py --batch_size 32 --num_workers 8 --num_iters 110000 --num_iters_decay 55000 --c_dim 8 --dataset duke --mode train --image_dir ../data/duke/bounding_box_train --log_dir ./duke/logs --model_save_dir ./duke/models --sample_dir ./duke/samples --result_dir ../data/duke/bounding_box_train_camstyle_stargan4reid --show_example 0</t>
+  </si>
+  <si>
+    <t>adopted</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">basis = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no_crop, -h 384,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> re 0.5</t>
+    </r>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=6,7 python3 examples/IDE.py --train -d dukemtmc  --combine-trainval --logs-dir logs/ide_new/256/basis_s_1/dukemtmc --height 384 --re 0.5 -s 1 --features 256 --output_feature fc</t>
+  </si>
+  <si>
+    <t>12fps</t>
+  </si>
+  <si>
+    <t>reid</t>
+  </si>
+  <si>
+    <t>mygt@12fps</t>
+  </si>
+  <si>
+    <t>mygt@30fps, single cam</t>
+  </si>
+  <si>
+    <t>#gpu</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>~10/sqrt(num_instance)</t>
+  </si>
+  <si>
+    <t>use smaller batch_size</t>
+  </si>
+  <si>
+    <t>imgs/GPU</t>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=2,3,4,5,6,7 python3 examples/IDE.py --lr 0.1 --epochs 20 -b 576 --train -d duke_my_gt --combine-trainval --logs-dir logs/ide_new/256/basis_s_1_crop/duke_my_gt/12_fps/lr01 --height 384 --re 0.5 -s 1 --features 256 --output_feature fc --mygt_fps 12 --crop</t>
+  </si>
+  <si>
+    <t>6fps</t>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=2,3,4,5,6,7 python3 examples/get_test_feature.py -b 576 --resume logs/ide_new/256/basis_s_1/duke_my_gt/checkpoint.pth.tar --features 256 --output_feature fc --l0_name my_gt_fc256 -s 1 --height 384 -d detections</t>
+  </si>
+  <si>
+    <t>1fps, 20epoch, 0.1lr, 96/GPU</t>
+  </si>
+  <si>
+    <t>12fps, 20epoch, 0.1lr, crop</t>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=2,3 python3 examples/IDE.py --lr 0.1 --epochs 20 -b 192 --train -d duke_my_gt --combine-trainval --logs-dir logs/ide_new/256/basis_s_1/duke_my_gt/1_fps/96_per_GPU --height 384 --re 0.5 -s 1 --features 256 --output_feature fc --mygt_fps 1</t>
+  </si>
+  <si>
+    <t>1fps, 20epoch, 0.1lr, 32/GPU</t>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=4,5,6,7 python3 examples/get_test_feature.py -j 16 -b 128 --resume logs/ide_new/256/basis_s_1_crop/duke_my_gt/12_fps/model_best.pth.tar --features 256 --output_feature fc --l0_name fc256_12fps_crop -s 1 --height 384 -d detections --det_time trainval_mini</t>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=2,3 python3 examples/IDE.py --lr 0.1 --epochs 20 -b 64 --train -d duke_my_gt --combine-trainval --logs-dir logs/ide_new/256/basis_s_1/duke_my_gt/1_fps/32_per_GPU --height 384 --re 0.5 -s 1 --features 256 --output_feature fc --mygt_fps 1</t>
+  </si>
+  <si>
+    <t>mygt@1fps</t>
+  </si>
+  <si>
+    <t>#imgs</t>
+  </si>
+  <si>
+    <t>#pids</t>
+  </si>
+  <si>
+    <t>mygt</t>
+  </si>
+  <si>
+    <t>iter</t>
+  </si>
+  <si>
+    <t>adpoted</t>
+  </si>
+  <si>
+    <t>CUDA_VISIBLE_DEVICES=4,5,6,7 python main.py --batch_size 128 --num_workers 16 --num_iters 110000 --num_iters_decay 50000 --g_lr 0.001 --d_lr 0.001 --c_dim 8 --dataset duke --mode train --image_dir /home/wangzd/Data/DukeMTMC/ALL_gt_bbox/gt_bbox_1_fps/allcam --log_dir ./duke_my_gt/logs --model_save_dir ./duke_my_gt/models --sample_dir ./duke_my_gt/samples --result_dir /home/wangzd/Data/DukeMTMC/ALL_gt_bbox/gt_bbox_1_fps/bounding_box_train_camstyle_stargan4reid --show_example 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1004,14 +1075,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1025,7 +1096,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1045,12 +1116,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1066,6 +1137,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1140,18 +1217,18 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1428,28 +1505,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="63.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.875" style="1"/>
+    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1457,7 +1534,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1468,7 +1545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1479,7 +1556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1490,7 +1567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1498,7 +1575,7 @@
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1506,7 +1583,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -1525,26 +1602,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="57.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1552,7 +1629,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1560,7 +1637,7 @@
         <v>0.72199999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1568,7 +1645,7 @@
         <v>0.752</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1576,13 +1653,13 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="14"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="16"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1590,7 +1667,7 @@
         <v>0.745</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1607,7 +1684,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1618,14 +1695,14 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1633,7 +1710,7 @@
         <v>0.74399999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1653,48 +1730,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1717,7 +1794,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>1501</v>
       </c>
@@ -1740,7 +1817,7 @@
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>1501</v>
       </c>
@@ -1760,7 +1837,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1783,7 +1860,7 @@
         <v>58.8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1806,7 +1883,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -1829,7 +1906,7 @@
         <v>69.7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1852,7 +1929,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -1875,7 +1952,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -1898,29 +1975,29 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
+    <row r="20" spans="1:8">
+      <c r="A20" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1937,7 +2014,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1954,7 +2031,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1983,26 +2060,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="7" max="7" width="66.75" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="66.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" thickBot="1">
       <c r="D2" t="s">
         <v>87</v>
       </c>
@@ -2010,7 +2087,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="19.8" thickBot="1">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -2021,7 +2098,7 @@
         <v>78.819999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="12" customHeight="1">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -2038,7 +2115,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>100</v>
       </c>
@@ -2049,7 +2126,7 @@
         <v>80.069999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2057,7 +2134,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
       <c r="D9" t="s">
         <v>21</v>
       </c>
@@ -2065,7 +2142,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -2076,7 +2153,7 @@
         <v>54.6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -2090,7 +2167,7 @@
         <v>71.3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -2107,7 +2184,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="D13">
         <v>62.05</v>
       </c>
@@ -2115,7 +2192,7 @@
         <v>76.77</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="B14" t="s">
         <v>97</v>
       </c>
@@ -2126,7 +2203,7 @@
         <v>78.11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="D15">
         <v>62.61</v>
       </c>
@@ -2134,7 +2211,7 @@
         <v>78.84</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
         <v>98</v>
       </c>
@@ -2145,7 +2222,7 @@
         <v>76.41</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7">
       <c r="B17" t="s">
         <v>103</v>
       </c>
@@ -2159,7 +2236,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7">
       <c r="C18" t="s">
         <v>106</v>
       </c>
@@ -2170,7 +2247,7 @@
         <v>66.48</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7">
       <c r="C19" t="s">
         <v>108</v>
       </c>
@@ -2181,12 +2258,12 @@
         <v>73.73</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7">
       <c r="C20" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7">
       <c r="B21" t="s">
         <v>111</v>
       </c>
@@ -2197,7 +2274,7 @@
         <v>72.8</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7">
       <c r="B22" t="s">
         <v>104</v>
       </c>
@@ -2208,7 +2285,7 @@
         <v>29.92</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7">
       <c r="B23" t="s">
         <v>107</v>
       </c>
@@ -2227,60 +2304,60 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:B48"/>
+    <sheetView topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.125" customWidth="1"/>
-    <col min="2" max="2" width="18.875" customWidth="1"/>
-    <col min="3" max="3" width="9.375" customWidth="1"/>
-    <col min="4" max="4" width="8.875" customWidth="1"/>
-    <col min="5" max="5" width="7.75" customWidth="1"/>
-    <col min="6" max="6" width="8.625" customWidth="1"/>
-    <col min="7" max="7" width="11.375" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="48.75" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="47.25" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="14" t="s">
+    <row r="6" spans="1:7" ht="54.75" customHeight="1"/>
+    <row r="7" spans="1:7">
+      <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="F7" s="14" t="s">
+      <c r="D7" s="16"/>
+      <c r="F7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="C8" t="s">
         <v>21</v>
       </c>
@@ -2294,7 +2371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="28.8">
       <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
@@ -2311,7 +2388,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="28.8">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -2331,7 +2408,7 @@
         <v>40.700000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="28.8">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
@@ -2351,7 +2428,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="43.2">
       <c r="A15" s="6" t="s">
         <v>35</v>
       </c>
@@ -2371,7 +2448,7 @@
         <v>42.4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="43.2">
       <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
@@ -2394,7 +2471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="57.6">
       <c r="A19" s="6" t="s">
         <v>37</v>
       </c>
@@ -2414,7 +2491,7 @@
         <v>42.9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="C20">
         <v>52</v>
       </c>
@@ -2428,7 +2505,7 @@
         <v>43.6</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="57.6">
       <c r="A22" s="6" t="s">
         <v>51</v>
       </c>
@@ -2448,7 +2525,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="57.6">
       <c r="A24" s="6" t="s">
         <v>52</v>
       </c>
@@ -2468,9 +2545,9 @@
         <v>42.3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="57.6">
       <c r="A26" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>55</v>
@@ -2488,7 +2565,7 @@
         <v>45.8</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="F27">
         <v>20.5</v>
       </c>
@@ -2502,7 +2579,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="C28">
         <v>52.5</v>
       </c>
@@ -2522,7 +2599,7 @@
         <v>69.099999999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="72">
       <c r="A30" s="8" t="s">
         <v>65</v>
       </c>
@@ -2548,13 +2625,13 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C33" s="14" t="s">
+    <row r="33" spans="1:9">
+      <c r="C33" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="14"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D33" s="16"/>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -2568,7 +2645,7 @@
         <v>73.819999999999993</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="B35" s="12" t="s">
         <v>117</v>
       </c>
@@ -2579,7 +2656,7 @@
         <v>74.03</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="B36" t="s">
         <v>116</v>
       </c>
@@ -2590,8 +2667,8 @@
         <v>73.180000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="17" t="s">
+    <row r="37" spans="1:9">
+      <c r="B37" s="14" t="s">
         <v>118</v>
       </c>
       <c r="C37">
@@ -2601,15 +2678,15 @@
         <v>78.81</v>
       </c>
       <c r="I37" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>126</v>
       </c>
       <c r="C38">
         <v>61.44</v>
@@ -2624,9 +2701,9 @@
         <v>39.840000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="17" t="s">
-        <v>148</v>
+    <row r="39" spans="1:9">
+      <c r="B39" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="C39">
         <v>59.37</v>
@@ -2641,9 +2718,9 @@
         <v>36.35</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="17" t="s">
-        <v>149</v>
+    <row r="40" spans="1:9">
+      <c r="B40" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="C40">
         <v>50.87</v>
@@ -2658,12 +2735,12 @@
         <v>43.71</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>120</v>
+      <c r="B41" s="15" t="s">
+        <v>164</v>
       </c>
       <c r="C41">
         <v>57.87</v>
@@ -2672,12 +2749,12 @@
         <v>76.38</v>
       </c>
       <c r="I41" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="B42" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="C42">
         <v>59.99</v>
@@ -2692,12 +2769,12 @@
         <v>36.380000000000003</v>
       </c>
       <c r="I42" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="B43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C43">
         <v>51.03</v>
@@ -2719,24 +2796,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="C2" t="s">
         <v>87</v>
       </c>
@@ -2744,7 +2821,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -2755,7 +2832,7 @@
         <v>74.09</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -2766,15 +2843,15 @@
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="C10" t="s">
         <v>21</v>
       </c>
@@ -2782,12 +2859,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C11">
         <v>90.98</v>
@@ -2795,61 +2872,109 @@
       <c r="D11">
         <v>97.56</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13">
+        <v>95.52</v>
+      </c>
+      <c r="D13">
+        <v>97.23</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14">
+        <v>97.16</v>
+      </c>
+      <c r="D14">
+        <v>99.15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15">
+        <v>96.67</v>
+      </c>
+      <c r="D15">
+        <v>99.06</v>
+      </c>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16">
+        <v>95.85</v>
+      </c>
+      <c r="D16">
+        <v>98.69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17">
+        <v>92.54</v>
+      </c>
+      <c r="D17">
+        <v>96.93</v>
+      </c>
+      <c r="F17" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>161</v>
-      </c>
-      <c r="C13">
-        <v>97.16</v>
-      </c>
-      <c r="D13">
-        <v>99.15</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14">
-        <v>96.67</v>
-      </c>
-      <c r="D14">
-        <v>99.06</v>
-      </c>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C15">
-        <v>95.85</v>
-      </c>
-      <c r="D15">
-        <v>98.69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16">
-        <v>92.54</v>
-      </c>
-      <c r="D16">
-        <v>96.93</v>
-      </c>
-      <c r="F16" t="s">
-        <v>156</v>
+    <row r="18" spans="2:6">
+      <c r="B18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18">
+        <v>84.13</v>
+      </c>
+      <c r="D18">
+        <v>92.36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19">
+        <v>83.54</v>
+      </c>
+      <c r="D19">
+        <v>91.29</v>
+      </c>
+      <c r="F19" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2860,57 +2985,57 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1.905</v>
       </c>
@@ -2930,11 +3055,11 @@
         <v>215279</v>
       </c>
       <c r="I3">
-        <f>(A3)*H3/3600</f>
+        <f t="shared" ref="I3:I8" si="0">(A3)*H3/3600</f>
         <v>113.91847083333333</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1.954</v>
       </c>
@@ -2954,11 +3079,11 @@
         <v>215279</v>
       </c>
       <c r="I4">
-        <f>(A4)*H4/3600</f>
+        <f t="shared" si="0"/>
         <v>116.84865722222222</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2.3090000000000002</v>
       </c>
@@ -2978,11 +3103,11 @@
         <v>35880</v>
       </c>
       <c r="I5">
-        <f>(A5)*H5/3600</f>
+        <f t="shared" si="0"/>
         <v>23.013033333333336</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>2.4430000000000001</v>
       </c>
@@ -3002,11 +3127,11 @@
         <v>26910</v>
       </c>
       <c r="I6">
-        <f>(A6)*H6/3600</f>
+        <f t="shared" si="0"/>
         <v>18.261425000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>2.3460000000000001</v>
       </c>
@@ -3026,11 +3151,11 @@
         <v>26910</v>
       </c>
       <c r="I7">
-        <f>(A7)*H7/3600</f>
+        <f t="shared" si="0"/>
         <v>17.536349999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>2.4279999999999999</v>
       </c>
@@ -3050,11 +3175,11 @@
         <v>17940</v>
       </c>
       <c r="I8">
-        <f>(A8)*H8/3600</f>
+        <f t="shared" si="0"/>
         <v>12.099533333333333</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>2.444</v>
       </c>
@@ -3078,7 +3203,7 @@
         <v>18.268899999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>2.798</v>
       </c>
@@ -3102,7 +3227,7 @@
         <v>10.457525</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>3.0129999999999999</v>
       </c>
@@ -3126,12 +3251,12 @@
         <v>11.2610875</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>2.9569999999999999</v>
       </c>
@@ -3151,11 +3276,11 @@
         <v>3686</v>
       </c>
       <c r="I16">
-        <f>(A16)*H16/3600</f>
+        <f t="shared" ref="I16:I24" si="1">(A16)*H16/3600</f>
         <v>3.0276394444444441</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>1.075</v>
       </c>
@@ -3175,11 +3300,11 @@
         <v>5529</v>
       </c>
       <c r="I17">
-        <f>(A17)*H17/3600</f>
+        <f t="shared" si="1"/>
         <v>1.6510208333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>0.9</v>
       </c>
@@ -3199,11 +3324,11 @@
         <v>11057</v>
       </c>
       <c r="I18">
-        <f>(A18)*H18/3600</f>
+        <f t="shared" si="1"/>
         <v>2.7642500000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>0.76100000000000001</v>
       </c>
@@ -3223,35 +3348,35 @@
         <v>11057</v>
       </c>
       <c r="I19">
-        <f>(A19)*H19/3600</f>
+        <f t="shared" si="1"/>
         <v>2.3373269444444444</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>0.70399999999999996</v>
       </c>
       <c r="B20">
         <v>0.38</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="9">
         <v>384</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="9">
         <v>16</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="9">
         <v>4</v>
       </c>
       <c r="H20">
         <v>6913</v>
       </c>
       <c r="I20">
-        <f>(A20)*H20/3600</f>
+        <f t="shared" si="1"/>
         <v>1.3518755555555555</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>0.78</v>
       </c>
@@ -3268,14 +3393,14 @@
         <v>4609</v>
       </c>
       <c r="I21">
-        <f>(A21)*H21/3600</f>
+        <f t="shared" si="1"/>
         <v>0.99861666666666671</v>
       </c>
       <c r="K21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3292,16 +3417,16 @@
         <v>16005</v>
       </c>
       <c r="I22">
-        <f>(A22)*H22/3600</f>
+        <f t="shared" si="1"/>
         <v>4.4458333333333337</v>
       </c>
       <c r="K22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <v>384</v>
@@ -3316,11 +3441,38 @@
         <v>6913</v>
       </c>
       <c r="I23">
-        <f>(A23)*H23/3600</f>
-        <v>1.9202777777777778</v>
+        <f t="shared" si="1"/>
+        <v>3.8405555555555555</v>
       </c>
       <c r="K23" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B24">
+        <v>0.38</v>
+      </c>
+      <c r="D24">
+        <v>384</v>
+      </c>
+      <c r="E24">
+        <v>16</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>20739</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>3.1684583333333336</v>
+      </c>
+      <c r="K24" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3331,47 +3483,50 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H1" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+      <c r="G1" t="s">
+        <v>174</v>
       </c>
       <c r="I1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2.1819999999999999</v>
       </c>
@@ -3387,18 +3542,22 @@
       <c r="F3">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="G3">
+        <f>D3/F3</f>
+        <v>128</v>
+      </c>
+      <c r="I3">
         <v>2487</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="J3">
-        <f>(A3)*H3/3600*I3</f>
+      <c r="K3">
+        <f t="shared" ref="K3:K14" si="0">(A3)*I3/3600*J3</f>
         <v>15.073983333333334</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>0.72199999999999998</v>
       </c>
@@ -3414,18 +3573,22 @@
       <c r="F4">
         <v>8</v>
       </c>
-      <c r="H4">
+      <c r="G4">
+        <f t="shared" ref="G4:G14" si="1">D4/F4</f>
+        <v>128</v>
+      </c>
+      <c r="I4">
         <v>1260</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>10</v>
       </c>
-      <c r="J4">
-        <f>(A4)*H4/3600*I4</f>
+      <c r="K4">
+        <f t="shared" si="0"/>
         <v>2.5269999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>0.67600000000000005</v>
       </c>
@@ -3441,18 +3604,22 @@
       <c r="F5">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="I5">
         <v>2016</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>10</v>
       </c>
-      <c r="J5">
-        <f>(A5)*H5/3600*I5</f>
+      <c r="K5">
+        <f t="shared" si="0"/>
         <v>3.7856000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>0.72199999999999998</v>
       </c>
@@ -3468,18 +3635,22 @@
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="H6">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="I6">
         <v>15926</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>10</v>
       </c>
-      <c r="J6">
-        <f>(A6)*H6/3600*I6</f>
+      <c r="K6">
+        <f t="shared" si="0"/>
         <v>31.940477777777776</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>0.72199999999999998</v>
       </c>
@@ -3495,18 +3666,22 @@
       <c r="F7">
         <v>6</v>
       </c>
-      <c r="H7">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="I7">
         <v>10000</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>6</v>
       </c>
-      <c r="J7">
-        <f>(A7)*H7/3600*I7</f>
+      <c r="K7">
+        <f t="shared" si="0"/>
         <v>12.033333333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>0.753</v>
       </c>
@@ -3522,18 +3697,22 @@
       <c r="F8">
         <v>8</v>
       </c>
-      <c r="H8">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="I8">
         <v>7963</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>6</v>
       </c>
-      <c r="J8">
-        <f>(A8)*H8/3600*I8</f>
+      <c r="K8">
+        <f t="shared" si="0"/>
         <v>9.9935650000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3546,15 +3725,303 @@
       <c r="F9">
         <v>3</v>
       </c>
-      <c r="H9">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="I9">
         <v>1415</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>20</v>
       </c>
-      <c r="J9">
-        <f>(A9)*H9/3600*I9</f>
+      <c r="K9">
+        <f t="shared" si="0"/>
         <v>7.8611111111111107</v>
+      </c>
+      <c r="M9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>576</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="I10">
+        <v>1415</v>
+      </c>
+      <c r="J10">
+        <v>20</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>7.8611111111111107</v>
+      </c>
+      <c r="M10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>1.071</v>
+      </c>
+      <c r="B11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D11">
+        <v>384</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="I11">
+        <v>2123</v>
+      </c>
+      <c r="J11">
+        <v>20</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>12.631849999999998</v>
+      </c>
+      <c r="M11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="B12">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D12">
+        <v>256</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <f>D12/F12</f>
+        <v>64</v>
+      </c>
+      <c r="I12">
+        <v>3185</v>
+      </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
+      <c r="K12">
+        <f>(A12)*I12/3600*J12</f>
+        <v>13.146972222222221</v>
+      </c>
+      <c r="M12" t="s">
+        <v>166</v>
+      </c>
+      <c r="N12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>0.433</v>
+      </c>
+      <c r="B13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D13">
+        <v>128</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I13">
+        <v>6370</v>
+      </c>
+      <c r="J13">
+        <v>20</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>15.323388888888889</v>
+      </c>
+      <c r="M13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="B14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D14">
+        <v>192</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I14">
+        <v>4246</v>
+      </c>
+      <c r="J14">
+        <v>20</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>10.048866666666667</v>
+      </c>
+      <c r="M14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="16:20">
+      <c r="Q21" t="s">
+        <v>167</v>
+      </c>
+      <c r="R21" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="S21" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="T21" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="16:20">
+      <c r="P22" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q22">
+        <v>702</v>
+      </c>
+      <c r="R22" s="14">
+        <v>1811</v>
+      </c>
+      <c r="S22" s="14">
+        <v>1812</v>
+      </c>
+      <c r="T22" s="14">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="23" spans="16:20">
+      <c r="P23" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q23">
+        <v>16522</v>
+      </c>
+      <c r="R23">
+        <v>67977</v>
+      </c>
+      <c r="S23">
+        <v>815417</v>
+      </c>
+      <c r="T23">
+        <v>330832</v>
+      </c>
+    </row>
+    <row r="24" spans="16:20">
+      <c r="Q24">
+        <f>1/SQRT(Q23)</f>
+        <v>7.7798046328871754E-3</v>
+      </c>
+      <c r="R24">
+        <f>1/SQRT(R23)</f>
+        <v>3.835473645373158E-3</v>
+      </c>
+      <c r="S24">
+        <f t="shared" ref="S24:T24" si="2">1/SQRT(S23)</f>
+        <v>1.1074142796483068E-3</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="2"/>
+        <v>1.7385862668511606E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="16:20">
+      <c r="P25" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q25">
+        <v>0.1</v>
+      </c>
+      <c r="R25">
+        <v>0.01</v>
+      </c>
+      <c r="S25">
+        <v>0.01</v>
+      </c>
+      <c r="T25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="16:20">
+      <c r="P26" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
+      </c>
+      <c r="S26">
+        <v>4</v>
+      </c>
+      <c r="T26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="16:20">
+      <c r="P27" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q27">
+        <v>64</v>
+      </c>
+      <c r="S27">
+        <v>128</v>
+      </c>
+      <c r="T27">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3562,4 +4029,311 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23AEED42-09A0-4D49-AAD6-17AEFE15C8CE}">
+  <dimension ref="A1:O20"/>
+  <sheetViews>
+    <sheetView zoomScale="68" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="12" max="12" width="34.88671875" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3">
+        <v>0.6</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>220000</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f>(A3)*G3*H3/3600</f>
+        <v>36.666666666666664</v>
+      </c>
+      <c r="J3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4">
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>220000</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f>(A4)*G4*H4/3600</f>
+        <v>30.555555555555557</v>
+      </c>
+      <c r="J4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="25.8" customHeight="1">
+      <c r="A5">
+        <v>0.7</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>110000</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f>(A5)*G5*H5/3600</f>
+        <v>21.388888888888889</v>
+      </c>
+      <c r="J5" t="s">
+        <v>167</v>
+      </c>
+      <c r="K5" t="s">
+        <v>163</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
+        <v>1.2</v>
+      </c>
+      <c r="C6">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>55000</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f>(A6)*G6*H6/3600</f>
+        <v>18.333333333333332</v>
+      </c>
+      <c r="J6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30.6" customHeight="1">
+      <c r="A9">
+        <v>0.8</v>
+      </c>
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>220000</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f>(A9)*G9*H9/3600</f>
+        <v>48.888888888888886</v>
+      </c>
+      <c r="J9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="33.6" customHeight="1">
+      <c r="A10">
+        <v>1.3</v>
+      </c>
+      <c r="C10">
+        <v>128</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>110000</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f>(A10)*G10*H10/3600</f>
+        <v>39.722222222222221</v>
+      </c>
+      <c r="J10" t="s">
+        <v>187</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="19.8" customHeight="1">
+      <c r="A11">
+        <v>1.3</v>
+      </c>
+      <c r="C11">
+        <v>192</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>80000</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f>(A11)*G11*H11/3600</f>
+        <v>28.888888888888889</v>
+      </c>
+      <c r="J11" t="s">
+        <v>187</v>
+      </c>
+      <c r="K11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="N15" t="s">
+        <v>167</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="M16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N16">
+        <v>702</v>
+      </c>
+      <c r="O16" s="14">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="17" spans="13:15">
+      <c r="M17" t="s">
+        <v>185</v>
+      </c>
+      <c r="N17">
+        <v>16522</v>
+      </c>
+      <c r="O17">
+        <v>67977</v>
+      </c>
+    </row>
+    <row r="18" spans="13:15">
+      <c r="M18" t="s">
+        <v>171</v>
+      </c>
+      <c r="N18">
+        <v>16</v>
+      </c>
+      <c r="O18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="13:15">
+      <c r="M19" t="s">
+        <v>188</v>
+      </c>
+      <c r="N19">
+        <v>220000</v>
+      </c>
+      <c r="O19">
+        <f>O20/O18</f>
+        <v>150907.67865068797</v>
+      </c>
+    </row>
+    <row r="20" spans="13:15">
+      <c r="N20">
+        <f>16*220000</f>
+        <v>3520000</v>
+      </c>
+      <c r="O20">
+        <f>16*220000/16522*67999</f>
+        <v>14487137.150466045</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>